<commit_message>
added the ability to export to pdf file
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Food</t>
   </si>
@@ -24,6 +24,18 @@
   </si>
   <si>
     <t>1500.0</t>
+  </si>
+  <si>
+    <t>walkdms</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>smws</t>
+  </si>
+  <si>
+    <t>1234.0</t>
   </si>
 </sst>
 </file>
@@ -68,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -88,6 +100,34 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
made the pdf that is exported open when it is exported
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>Food</t>
   </si>
@@ -26,6 +26,18 @@
     <t>1500.0</t>
   </si>
   <si>
+    <t>dfgh</t>
+  </si>
+  <si>
+    <t>3456.0</t>
+  </si>
+  <si>
+    <t>ghj</t>
+  </si>
+  <si>
+    <t>-678.0</t>
+  </si>
+  <si>
     <t>walkdms</t>
   </si>
   <si>
@@ -36,6 +48,78 @@
   </si>
   <si>
     <t>1234.0</t>
+  </si>
+  <si>
+    <t>Atb Kort</t>
+  </si>
+  <si>
+    <t>234.0</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>123.0</t>
+  </si>
+  <si>
+    <t>wqer</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>hjk</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>buss</t>
+  </si>
+  <si>
+    <t>145.0</t>
+  </si>
+  <si>
+    <t>taxi</t>
+  </si>
+  <si>
+    <t>300.0</t>
+  </si>
+  <si>
+    <t>Rent</t>
+  </si>
+  <si>
+    <t>campus</t>
+  </si>
+  <si>
+    <t>7000.0</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>gucci</t>
+  </si>
+  <si>
+    <t>2023-03-09</t>
+  </si>
+  <si>
+    <t>4000.0</t>
+  </si>
+  <si>
+    <t>atb</t>
+  </si>
+  <si>
+    <t>Maxi Taxi</t>
+  </si>
+  <si>
+    <t>6000.0</t>
   </si>
 </sst>
 </file>
@@ -80,7 +164,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -111,12 +195,12 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -126,6 +210,188 @@
       </c>
       <c r="D3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed text from excell to pdf on button
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
   <si>
     <t>Food</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>6000.0</t>
+  </si>
+  <si>
+    <t>food</t>
   </si>
 </sst>
 </file>
@@ -164,7 +167,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -394,6 +397,20 @@
         <v>35</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Moved all windows from GUI-class to separate classes
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
   <si>
     <t>Food</t>
   </si>
@@ -132,6 +132,24 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>fae</t>
+  </si>
+  <si>
+    <t>tset</t>
+  </si>
+  <si>
+    <t>344.0</t>
+  </si>
+  <si>
+    <t>halla</t>
+  </si>
+  <si>
+    <t>rtyu</t>
+  </si>
+  <si>
+    <t>5678.0</t>
   </si>
 </sst>
 </file>
@@ -176,7 +194,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -448,6 +466,62 @@
         <v>15</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
made topmenu larger and implemented them to their respective windows
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="48">
   <si>
     <t>Food</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>5678.0</t>
+  </si>
+  <si>
+    <t>123423</t>
+  </si>
+  <si>
+    <t>124.0</t>
   </si>
 </sst>
 </file>
@@ -194,7 +200,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -522,6 +528,20 @@
         <v>45</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
left piechart now updates automatically when a new expense is added, each account has an arraylist that consists of each added expense, this is also added to the bank statement
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="63">
   <si>
     <t>Food</t>
   </si>
@@ -156,6 +156,51 @@
   </si>
   <si>
     <t>124.0</t>
+  </si>
+  <si>
+    <t>sdfg</t>
+  </si>
+  <si>
+    <t>10000.0</t>
+  </si>
+  <si>
+    <t>dgrdgf</t>
+  </si>
+  <si>
+    <t>2023-03-11</t>
+  </si>
+  <si>
+    <t>adms</t>
+  </si>
+  <si>
+    <t>150.0</t>
+  </si>
+  <si>
+    <t>dfms</t>
+  </si>
+  <si>
+    <t>asws</t>
+  </si>
+  <si>
+    <t>KSLKFVASZ</t>
+  </si>
+  <si>
+    <t>99.0</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>gthfthfg</t>
+  </si>
+  <si>
+    <t>4999.0</t>
+  </si>
+  <si>
+    <t>gtfg</t>
+  </si>
+  <si>
+    <t>545.0</t>
   </si>
 </sst>
 </file>
@@ -200,7 +245,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -542,6 +587,127 @@
         <v>47</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>